<commit_message>
Added some more stuff. And Fixed the other
</commit_message>
<xml_diff>
--- a/Stocks.xlsx
+++ b/Stocks.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rosscuttriss/Desktop/Grafana/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D73EFF18-1B22-F645-BA34-41683B32D771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C7E24D-DCA7-0D47-B9F3-F401F6D0DC5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="500" windowWidth="24460" windowHeight="16040" xr2:uid="{D7BE4A4B-A1DD-5545-90DD-63D7073E3D33}"/>
+    <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="16040" activeTab="1" xr2:uid="{D7BE4A4B-A1DD-5545-90DD-63D7073E3D33}"/>
   </bookViews>
   <sheets>
     <sheet name="Stocks" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -133,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Stock</t>
   </si>
@@ -154,6 +155,27 @@
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t>Meta Platforms</t>
+  </si>
+  <si>
+    <t>DEERE &amp; COMPANY</t>
+  </si>
+  <si>
+    <t>TESLA</t>
+  </si>
+  <si>
+    <t>AIRBNB</t>
+  </si>
+  <si>
+    <t>MICROSOFT</t>
+  </si>
+  <si>
+    <t>APPLE</t>
+  </si>
+  <si>
+    <t>GM</t>
   </si>
 </sst>
 </file>
@@ -383,7 +405,7 @@
     <v>2549405000</v>
     <v>META</v>
     <v>Meta Platforms, Inc. (XNAS:META)</v>
-    <v>112987</v>
+    <v>145173</v>
     <v>13920479</v>
     <v>2004</v>
   </rv>
@@ -434,7 +456,7 @@
     <v>278358200</v>
     <v>DE</v>
     <v>DEERE &amp; COMPANY (XNYS:DE)</v>
-    <v>118</v>
+    <v>249</v>
     <v>1381515</v>
     <v>1958</v>
   </rv>
@@ -485,7 +507,7 @@
     <v>3184791000</v>
     <v>TSLA</v>
     <v>TESLA, INC. (XNAS:TSLA)</v>
-    <v>818179</v>
+    <v>1026954</v>
     <v>95584224</v>
     <v>2003</v>
   </rv>
@@ -536,7 +558,7 @@
     <v>647064700</v>
     <v>ABNB</v>
     <v>AIRBNB, INC. (XNAS:ABNB)</v>
-    <v>8107</v>
+    <v>15781</v>
     <v>3782213</v>
     <v>2008</v>
   </rv>
@@ -608,7 +630,7 @@
     <v>7430436000</v>
     <v>MSFT</v>
     <v>MICROSOFT CORPORATION (XNAS:MSFT)</v>
-    <v>107740</v>
+    <v>145494</v>
     <v>19575440</v>
     <v>1993</v>
   </rv>
@@ -659,7 +681,7 @@
     <v>15441880000</v>
     <v>AAPL</v>
     <v>APPLE INC. (XNAS:AAPL)</v>
-    <v>741232</v>
+    <v>898828</v>
     <v>62963430</v>
     <v>1977</v>
   </rv>
@@ -710,7 +732,7 @@
     <v>1154433000</v>
     <v>GM</v>
     <v>GENERAL MOTORS COMPANY (XNYS:GM)</v>
-    <v>6342</v>
+    <v>7633</v>
     <v>17414749</v>
     <v>2009</v>
   </rv>
@@ -1485,8 +1507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34EC763F-1745-D64C-B690-784AB1AE9E6E}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1736,4 +1758,254 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B63BC49-66A5-AF4F-ABAF-8134BE2E190C}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <f>Stocks!B2</f>
+        <v>531.48990000000003</v>
+      </c>
+      <c r="C2" s="1">
+        <f>Stocks!C2</f>
+        <v>207.13</v>
+      </c>
+      <c r="D2" s="1">
+        <f>Stocks!D2</f>
+        <v>3.33</v>
+      </c>
+      <c r="E2" s="2">
+        <f>Stocks!E2</f>
+        <v>6.4059999999999994E-3</v>
+      </c>
+      <c r="F2" t="str">
+        <f>Stocks!F2</f>
+        <v>USD</v>
+      </c>
+      <c r="G2" s="1">
+        <f>Stocks!G2</f>
+        <v>523.16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1">
+        <f>Stocks!B3</f>
+        <v>450</v>
+      </c>
+      <c r="C3" s="1">
+        <f>Stocks!C3</f>
+        <v>345.55</v>
+      </c>
+      <c r="D3" s="1">
+        <f>Stocks!D3</f>
+        <v>0.87</v>
+      </c>
+      <c r="E3" s="2">
+        <f>Stocks!E3</f>
+        <v>2.1120000000000002E-3</v>
+      </c>
+      <c r="F3" t="str">
+        <f>Stocks!F3</f>
+        <v>USD</v>
+      </c>
+      <c r="G3" s="1">
+        <f>Stocks!G3</f>
+        <v>412.84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1">
+        <f>Stocks!B4</f>
+        <v>299.29000000000002</v>
+      </c>
+      <c r="C4" s="1">
+        <f>Stocks!C4</f>
+        <v>152.37</v>
+      </c>
+      <c r="D4" s="1">
+        <f>Stocks!D4</f>
+        <v>2.84</v>
+      </c>
+      <c r="E4" s="2">
+        <f>Stocks!E4</f>
+        <v>1.6535000000000001E-2</v>
+      </c>
+      <c r="F4" t="str">
+        <f>Stocks!F4</f>
+        <v>USD</v>
+      </c>
+      <c r="G4" s="1">
+        <f>Stocks!G4</f>
+        <v>174.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1">
+        <f>Stocks!B5</f>
+        <v>170.1</v>
+      </c>
+      <c r="C5" s="1">
+        <f>Stocks!C5</f>
+        <v>103.55</v>
+      </c>
+      <c r="D5" s="1">
+        <f>Stocks!D5</f>
+        <v>5.14</v>
+      </c>
+      <c r="E5" s="2">
+        <f>Stocks!E5</f>
+        <v>3.2069E-2</v>
+      </c>
+      <c r="F5" t="str">
+        <f>Stocks!F5</f>
+        <v>USD</v>
+      </c>
+      <c r="G5" s="1">
+        <f>Stocks!G5</f>
+        <v>165.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1">
+        <f>Stocks!B6</f>
+        <v>430.82</v>
+      </c>
+      <c r="C6" s="1">
+        <f>Stocks!C6</f>
+        <v>275.37</v>
+      </c>
+      <c r="D6" s="1">
+        <f>Stocks!D6</f>
+        <v>4.67</v>
+      </c>
+      <c r="E6" s="2">
+        <f>Stocks!E6</f>
+        <v>1.1032999999999999E-2</v>
+      </c>
+      <c r="F6" t="str">
+        <f>Stocks!F6</f>
+        <v>USD</v>
+      </c>
+      <c r="G6" s="1">
+        <f>Stocks!G6</f>
+        <v>427.93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <f>Stocks!B7</f>
+        <v>199.62</v>
+      </c>
+      <c r="C7" s="1">
+        <f>Stocks!C7</f>
+        <v>159.78</v>
+      </c>
+      <c r="D7" s="1">
+        <f>Stocks!D7</f>
+        <v>7.26</v>
+      </c>
+      <c r="E7" s="2">
+        <f>Stocks!E7</f>
+        <v>4.3270999999999997E-2</v>
+      </c>
+      <c r="F7" t="str">
+        <f>Stocks!F7</f>
+        <v>USD</v>
+      </c>
+      <c r="G7" s="1">
+        <f>Stocks!G7</f>
+        <v>175.04</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1">
+        <f>Stocks!B8</f>
+        <v>46.04</v>
+      </c>
+      <c r="C8" s="1">
+        <f>Stocks!C8</f>
+        <v>26.3</v>
+      </c>
+      <c r="D8" s="1">
+        <f>Stocks!D8</f>
+        <v>-0.1</v>
+      </c>
+      <c r="E8" s="2">
+        <f>Stocks!E8</f>
+        <v>-2.2759999999999998E-3</v>
+      </c>
+      <c r="F8" t="str">
+        <f>Stocks!F8</f>
+        <v>USD</v>
+      </c>
+      <c r="G8" s="1">
+        <f>Stocks!G8</f>
+        <v>43.84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>